<commit_message>
PAR code and edited txt files from PAR sensors
</commit_message>
<xml_diff>
--- a/Documents/1_ocean_acidification/0_metadata_summer_school.xlsx
+++ b/Documents/1_ocean_acidification/0_metadata_summer_school.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://publicadministrationis-my.sharepoint.com/personal/einar_petur_jonsson_hafogvatn_is/Documents/Documents/surt/BOAT/Ischia/R_Git/nuriateixidolab/nuriateixidolab.github.io/Documents/1_ocean_acidification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{448B0612-8E0C-4DB6-901A-9716605ECC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EC3BC7E7-5225-F749-9354-F6FBA83BA62E}"/>
+  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:1_{448B0612-8E0C-4DB6-901A-9716605ECC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C854DAA2-A982-2E40-AD78-747ADED6C987}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="12220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>sensor_id</t>
   </si>
@@ -95,6 +95,18 @@
   </si>
   <si>
     <t>tris_calibration</t>
+  </si>
+  <si>
+    <t>22068746 2025-09-16_hobo2_tris</t>
+  </si>
+  <si>
+    <t>22068746 2025-09-16_hobo2</t>
+  </si>
+  <si>
+    <t>22068747 2025-09-16_hobo3_tris</t>
+  </si>
+  <si>
+    <t>22068747 2025-09-16_hobo3</t>
   </si>
 </sst>
 </file>
@@ -236,6 +248,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,7 +458,7 @@
   <dimension ref="A1:R1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -453,6 +469,7 @@
     <col min="12" max="12" width="20.33203125" customWidth="1"/>
     <col min="13" max="13" width="15.6640625" customWidth="1"/>
     <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1">
@@ -545,7 +562,9 @@
       <c r="K2" s="1">
         <v>1</v>
       </c>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" ht="16">
@@ -582,6 +601,9 @@
       <c r="K3" s="1">
         <v>5</v>
       </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" ht="16">
@@ -618,6 +640,9 @@
       <c r="K4" s="1">
         <v>1</v>
       </c>
+      <c r="Q4" t="s">
+        <v>27</v>
+      </c>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" ht="16">
@@ -654,7 +679,9 @@
       <c r="K5" s="1">
         <v>5</v>
       </c>
-      <c r="Q5" s="1"/>
+      <c r="Q5" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" ht="13">

</xml_diff>